<commit_message>
now dynamically finds correct column to enter time into
</commit_message>
<xml_diff>
--- a/template/G Network_Network_Projects_Timesheet v0.1.xlsx
+++ b/template/G Network_Network_Projects_Timesheet v0.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\marco\projects\timesheet\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063E9B56-91B7-4251-B265-3C67AC69C293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CFAC21-ED1D-4E20-BDA3-5C2C92EB55FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-9720" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,9 +58,6 @@
     <t>10 G &amp; Spitfire</t>
   </si>
   <si>
-    <t>System Review</t>
-  </si>
-  <si>
     <t>Network  &amp; System Monitoring</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>Manager</t>
+  </si>
+  <si>
+    <t>System-Review</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1031,7 @@
   <dimension ref="B1:AE32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,50 +1096,50 @@
         <v>6</v>
       </c>
       <c r="T4" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="U4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="U4" s="25" t="s">
+      <c r="V4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="V4" s="25" t="s">
+      <c r="W4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="W4" s="24" t="s">
+      <c r="X4" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="25" t="s">
+      <c r="Y4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="Y4" s="25" t="s">
+      <c r="Z4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Z4" s="25" t="s">
+      <c r="AA4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="25" t="s">
+      <c r="AB4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="AB4" s="25" t="s">
+      <c r="AC4" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="AC4" s="25" t="s">
+      <c r="AD4" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="25" t="s">
+      <c r="AE4" s="26" t="s">
         <v>17</v>
-      </c>
-      <c r="AE4" s="26" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5"/>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K5" s="6"/>
       <c r="M5" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N5" s="18"/>
       <c r="O5" s="18"/>
@@ -1234,7 +1234,7 @@
     <row r="9" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
       <c r="I9" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J9" s="16"/>
       <c r="K9" s="17"/>
@@ -1261,7 +1261,7 @@
     <row r="10" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="39"/>
       <c r="E10" s="40"/>
@@ -1385,19 +1385,19 @@
     <row r="15" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="E15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="F15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="H15" s="42" t="s">
         <v>26</v>
-      </c>
-      <c r="H15" s="42" t="s">
-        <v>27</v>
       </c>
       <c r="I15" s="42"/>
       <c r="J15" s="42"/>
@@ -1437,7 +1437,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I16" s="43"/>
       <c r="J16" s="43"/>
@@ -1477,7 +1477,7 @@
         <v>0</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I17" s="43"/>
       <c r="J17" s="43"/>
@@ -1517,7 +1517,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I18" s="43"/>
       <c r="J18" s="43"/>
@@ -1731,10 +1731,10 @@
     <row r="25" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="5"/>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K25" s="6"/>
       <c r="M25" s="20"/>
@@ -1812,10 +1812,10 @@
     <row r="28" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="5"/>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K28" s="6"/>
       <c r="M28" s="20"/>

</xml_diff>